<commit_message>
This my six commit
</commit_message>
<xml_diff>
--- a/Test_data/datafile.xlsx
+++ b/Test_data/datafile.xlsx
@@ -1,92 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Harshal data\pythonProject\pythonProject2\Test_data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97A56D7-4AC1-4A79-A5D8-E63DE1DD8914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="User" sheetId="1" r:id="rId1"/>
+    <sheet name="User" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>hbhagat505@gmail.com</t>
-  </si>
-  <si>
-    <t>ramesh@Gmail.com</t>
-  </si>
-  <si>
-    <t>Pass@245</t>
-  </si>
-  <si>
-    <t>suresh@gmail.com</t>
-  </si>
-  <si>
-    <t>Pass@298</t>
-  </si>
-  <si>
-    <t>jayesh@gmail.com</t>
-  </si>
-  <si>
-    <t>pass@289</t>
-  </si>
-  <si>
-    <t>12345@</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.8"/>
-      <color rgb="FF808080"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <color rgb="FF808080"/>
+      <sz val="12.8"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -103,29 +58,88 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -391,71 +405,166 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col width="21" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="12.77734375" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.8">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
+    <row r="1" ht="16.8" customHeight="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Password</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Expected</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Actual</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>ramesh@Gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Pass@245</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="E2">
+        <f>C2=D2</f>
+        <v/>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>suresh@gmail.com</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>Pass@298</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="E3">
+        <f>C3=D3</f>
+        <v/>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>jayesh@gmail.com</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>pass@289</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="E4">
+        <f>C4=D4</f>
+        <v/>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>hbhagat505@gmail.com</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>12345@</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E5">
+        <f>C5=D5</f>
+        <v/>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" xr:uid="{04DFE41F-9FF7-4D6B-83D8-E051B8732086}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{DEED84C1-0F0A-41E7-B45D-6666324CECB8}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{97A3C231-4B0F-4106-A3B9-0BB256CD6254}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{891FED9E-2614-4A83-AE30-A05B6EDDB008}"/>
-    <hyperlink ref="A3" r:id="rId5" xr:uid="{ECA24292-E06E-4E26-9A65-8AC92D2B7D38}"/>
-    <hyperlink ref="B3" r:id="rId6" xr:uid="{120301F3-00AA-49AF-912A-35592DEFDE47}"/>
-    <hyperlink ref="A4" r:id="rId7" xr:uid="{ADD3F113-6369-4160-B696-4FD19F7D8D31}"/>
-    <hyperlink ref="B4" r:id="rId8" xr:uid="{CDF6D3D6-1C6B-47D3-8B68-3C62F0B008F1}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
+    <hyperlink ref="B4" r:id="rId6"/>
+    <hyperlink ref="A5" r:id="rId7"/>
+    <hyperlink ref="B5" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>